<commit_message>
Complete run and updated .gitignore to exclude Adobe Illustrator formatted figures
</commit_message>
<xml_diff>
--- a/output_data/OBER_proj3_Q15250_Mn_oxidation_heatmap_data_genus_table_1pct.xlsx
+++ b/output_data/OBER_proj3_Q15250_Mn_oxidation_heatmap_data_genus_table_1pct.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">tax_label</t>
   </si>
@@ -38,36 +38,24 @@
     <t xml:space="preserve">*A0839*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Afipia*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Amb-16S-1323*</t>
   </si>
   <si>
     <t xml:space="preserve">*Amphiplicatus*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Arenimonas*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Bacillus*</t>
   </si>
   <si>
     <t xml:space="preserve">*Brevibacillus*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Bryobacter*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Candidatus_Accumulibacter*</t>
   </si>
   <si>
     <t xml:space="preserve">*Candidatus_Adlerbacteria*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Chryseobacterium*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Ellin6067*</t>
   </si>
   <si>
@@ -83,9 +71,6 @@
     <t xml:space="preserve">*Gemmata*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Hirschia*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Hoeflea*</t>
   </si>
   <si>
@@ -95,18 +80,9 @@
     <t xml:space="preserve">*Hyphomicrobium*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Luteimonas*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*MND1*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Mycobacterium*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*NS9_marine_group*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Nevskia*</t>
   </si>
   <si>
@@ -116,15 +92,9 @@
     <t xml:space="preserve">*Nitrospira*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Novosphingobium*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Pedomicrobium*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Phenylobacterium*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Pir4_lineage*</t>
   </si>
   <si>
@@ -134,9 +104,6 @@
     <t xml:space="preserve">*Planctopirus*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Pseudolabrys*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Pseudomonas*</t>
   </si>
   <si>
@@ -146,12 +113,6 @@
     <t xml:space="preserve">*Reyranella*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Rhizobacter*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Rhodobacter*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Rhodococcus*</t>
   </si>
   <si>
@@ -170,21 +131,12 @@
     <t xml:space="preserve">*Sphingorhabdus*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Stenotrophobacter*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Terrimonas*</t>
   </si>
   <si>
-    <t xml:space="preserve">*Undibacterium*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Vicinamibacteraceae*</t>
   </si>
   <si>
-    <t xml:space="preserve">*env.OPS_17*</t>
-  </si>
-  <si>
     <t xml:space="preserve">Genus of Blastocatellaceae</t>
   </si>
   <si>
@@ -194,6 +146,9 @@
     <t xml:space="preserve">Genus of Comamonadaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Genus of Gallionellaceae</t>
+  </si>
+  <si>
     <t xml:space="preserve">Genus of Gemmataceae</t>
   </si>
   <si>
@@ -209,7 +164,16 @@
     <t xml:space="preserve">Genus of Planctomycetales</t>
   </si>
   <si>
+    <t xml:space="preserve">Genus of Rhizobiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genus of Rhizobiales</t>
+  </si>
+  <si>
     <t xml:space="preserve">Genus of Rhizobiales_Incertae_Sedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genus of Rhodobacteraceae</t>
   </si>
   <si>
     <t xml:space="preserve">Genus of Rubinisphaeraceae</t>
@@ -590,22 +554,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>3.99478360653786</v>
+        <v>3.73952943844442</v>
       </c>
       <c r="C2" t="n">
-        <v>4.10205514821947</v>
+        <v>3.80486036079433</v>
       </c>
       <c r="D2" t="n">
-        <v>1.17013437985563</v>
+        <v>1.08876313168077</v>
       </c>
       <c r="E2" t="n">
-        <v>3.01035559408455</v>
+        <v>2.80297064767523</v>
       </c>
       <c r="F2" t="n">
-        <v>2.28244717868126</v>
+        <v>2.1494760261845</v>
       </c>
       <c r="G2" t="n">
-        <v>0.429757954975617</v>
+        <v>0.399230498727841</v>
       </c>
     </row>
     <row r="3">
@@ -613,22 +577,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.614294255276114</v>
+        <v>1.45338949997499</v>
       </c>
       <c r="C3" t="n">
-        <v>0.579523393024137</v>
+        <v>1.44588853319575</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0762324250474947</v>
+        <v>0.131312958963634</v>
       </c>
       <c r="E3" t="n">
-        <v>1.10124772235201</v>
+        <v>1.2794408208258</v>
       </c>
       <c r="F3" t="n">
-        <v>0.765675908077906</v>
+        <v>0.75407390237415</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0935224565231913</v>
+        <v>0.21099228430176</v>
       </c>
     </row>
     <row r="4">
@@ -636,22 +600,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>2.06310822988118</v>
+        <v>0.0817240278917347</v>
       </c>
       <c r="C4" t="n">
-        <v>1.92692354267361</v>
+        <v>0.115841856917132</v>
       </c>
       <c r="D4" t="n">
-        <v>0.146937997386338</v>
+        <v>0.0413585242313299</v>
       </c>
       <c r="E4" t="n">
-        <v>1.94608871243509</v>
+        <v>0.8315864533156</v>
       </c>
       <c r="F4" t="n">
-        <v>1.26538512532451</v>
+        <v>0.87510207204443</v>
       </c>
       <c r="G4" t="n">
-        <v>0.233806141307978</v>
+        <v>0.0599880023995201</v>
       </c>
     </row>
     <row r="5">
@@ -659,22 +623,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0873182876956604</v>
+        <v>0.351693567708582</v>
       </c>
       <c r="C5" t="n">
-        <v>0.124745621403874</v>
+        <v>0.755069652410652</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0441980925762741</v>
+        <v>0.345341897304699</v>
       </c>
       <c r="E5" t="n">
-        <v>0.891822019958815</v>
+        <v>0.403380332533456</v>
       </c>
       <c r="F5" t="n">
-        <v>0.929206591707898</v>
+        <v>0.993062787239732</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0645750295041083</v>
+        <v>0.597811472188321</v>
       </c>
     </row>
     <row r="6">
@@ -682,22 +646,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.136960850609055</v>
+        <v>0.295831876291526</v>
       </c>
       <c r="C6" t="n">
-        <v>0.145952922632514</v>
+        <v>0.669227231465924</v>
       </c>
       <c r="D6" t="n">
-        <v>0.943583606079743</v>
+        <v>0.274000129487603</v>
       </c>
       <c r="E6" t="n">
-        <v>0.38427256039541</v>
+        <v>0.23271937406331</v>
       </c>
       <c r="F6" t="n">
-        <v>0.34161565886357</v>
+        <v>0.921690752847712</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0912957313678773</v>
+        <v>0.409573257762241</v>
       </c>
     </row>
     <row r="7">
@@ -705,22 +669,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>0.375586522862194</v>
+        <v>0.0548260884981641</v>
       </c>
       <c r="C7" t="n">
-        <v>0.812698017113733</v>
+        <v>0.0672278501642858</v>
       </c>
       <c r="D7" t="n">
-        <v>0.36899836513242</v>
+        <v>0.0599694806101723</v>
       </c>
       <c r="E7" t="n">
-        <v>0.432970598207991</v>
+        <v>1.12015281067438</v>
       </c>
       <c r="F7" t="n">
-        <v>1.05398987332298</v>
+        <v>0.701309867751208</v>
       </c>
       <c r="G7" t="n">
-        <v>0.643523569885769</v>
+        <v>0.02895972529632</v>
       </c>
     </row>
     <row r="8">
@@ -728,22 +692,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.315902751411982</v>
+        <v>0.854290076059088</v>
       </c>
       <c r="C8" t="n">
-        <v>0.720191993452507</v>
+        <v>0.348537811683693</v>
       </c>
       <c r="D8" t="n">
-        <v>0.292809435726552</v>
+        <v>0.00310173697270471</v>
       </c>
       <c r="E8" t="n">
-        <v>0.249806284893106</v>
+        <v>0.053783502309325</v>
       </c>
       <c r="F8" t="n">
-        <v>0.978186663341064</v>
+        <v>0.0362048991950056</v>
       </c>
       <c r="G8" t="n">
-        <v>0.440891580752188</v>
+        <v>0.02482262168256</v>
       </c>
     </row>
     <row r="9">
@@ -751,22 +715,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.70064152215854</v>
+        <v>3.35680399470763</v>
       </c>
       <c r="C9" t="n">
-        <v>0.721188018150731</v>
+        <v>3.54338414746873</v>
       </c>
       <c r="D9" t="n">
-        <v>0.855381478405224</v>
+        <v>0.894377137689368</v>
       </c>
       <c r="E9" t="n">
-        <v>0.740820351940616</v>
+        <v>3.8114281224236</v>
       </c>
       <c r="F9" t="n">
-        <v>0.630487520522263</v>
+        <v>2.65115145084603</v>
       </c>
       <c r="G9" t="n">
-        <v>0.999799594736022</v>
+        <v>0.333036840907681</v>
       </c>
     </row>
     <row r="10">
@@ -774,22 +738,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0585705130249587</v>
+        <v>0.742746210001179</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0724203620191666</v>
+        <v>0.806742930399453</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0640753565796146</v>
+        <v>6.66287836316038</v>
       </c>
       <c r="E10" t="n">
-        <v>1.27007348815668</v>
+        <v>0.419928597203309</v>
       </c>
       <c r="F10" t="n">
-        <v>0.784374462729104</v>
+        <v>0.42203468275203</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0311741521743971</v>
+        <v>1.64656723827648</v>
       </c>
     </row>
     <row r="11">
@@ -797,22 +761,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>0.911613506372715</v>
+        <v>0.0641295646863152</v>
       </c>
       <c r="C11" t="n">
-        <v>0.375637013074009</v>
+        <v>0.125139686510327</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00331008915173449</v>
+        <v>0.607971557030266</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0579030684145479</v>
+        <v>0.0899845496296847</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0384323546283958</v>
+        <v>0.235840241059572</v>
       </c>
       <c r="G11" t="n">
-        <v>0.026720701863769</v>
+        <v>1.06737273235008</v>
       </c>
     </row>
     <row r="12">
@@ -820,22 +784,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>0.00220463414096431</v>
+        <v>0.10137120593653</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00667319156508586</v>
+        <v>0.0889471527433076</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>4.54532585674994</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00996236440115121</v>
+        <v>0.103431206155929</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00768318918206963</v>
+        <v>0.13033643873551</v>
       </c>
       <c r="G12" t="n">
-        <v>1.04656082299762</v>
+        <v>4.36671286432369</v>
       </c>
     </row>
     <row r="13">
@@ -843,22 +807,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>3.58605645275519</v>
+        <v>0.182061171825907</v>
       </c>
       <c r="C13" t="n">
-        <v>3.81763834533121</v>
+        <v>0.231678258566748</v>
       </c>
       <c r="D13" t="n">
-        <v>0.95575405782197</v>
+        <v>0.0940897633036752</v>
       </c>
       <c r="E13" t="n">
-        <v>4.09065366946349</v>
+        <v>1.16463358534722</v>
       </c>
       <c r="F13" t="n">
-        <v>2.81524023238675</v>
+        <v>0.926812164721499</v>
       </c>
       <c r="G13" t="n">
-        <v>0.358502750005567</v>
+        <v>0.444738638479201</v>
       </c>
     </row>
     <row r="14">
@@ -866,22 +830,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>0.79352063130308</v>
+        <v>0.112754363003401</v>
       </c>
       <c r="C14" t="n">
-        <v>0.868931052321197</v>
+        <v>0.0899852152751762</v>
       </c>
       <c r="D14" t="n">
-        <v>7.12094206251392</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.450948806049975</v>
+        <v>0.379589996959657</v>
       </c>
       <c r="F14" t="n">
-        <v>0.448131935112107</v>
+        <v>1.00543191976414</v>
       </c>
       <c r="G14" t="n">
-        <v>1.77247322363001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -889,22 +853,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0684694839497567</v>
+        <v>0.153098190260689</v>
       </c>
       <c r="C15" t="n">
-        <v>0.134911185126106</v>
+        <v>0.393000659362568</v>
       </c>
       <c r="D15" t="n">
-        <v>0.649751106948694</v>
+        <v>0.0713434783534616</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0966798707175922</v>
+        <v>3.54353061574049</v>
       </c>
       <c r="F15" t="n">
-        <v>0.250455915748345</v>
+        <v>4.29891580178209</v>
       </c>
       <c r="G15" t="n">
-        <v>1.14899018014206</v>
+        <v>0.14273007467472</v>
       </c>
     </row>
     <row r="16">
@@ -912,22 +876,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>0.108262312034821</v>
+        <v>4.38498213569021</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0958237374589683</v>
+        <v>5.83101878954667</v>
       </c>
       <c r="D16" t="n">
-        <v>4.85812284873267</v>
+        <v>0.979162759160157</v>
       </c>
       <c r="E16" t="n">
-        <v>0.110905437063909</v>
+        <v>3.90244645585104</v>
       </c>
       <c r="F16" t="n">
-        <v>0.138369603636663</v>
+        <v>4.39616992065702</v>
       </c>
       <c r="G16" t="n">
-        <v>4.70061680286802</v>
+        <v>1.92789028401216</v>
       </c>
     </row>
     <row r="17">
@@ -935,22 +899,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>0.19447828266</v>
+        <v>0.458245099614371</v>
       </c>
       <c r="C17" t="n">
-        <v>0.249562050250749</v>
+        <v>0.960800711894697</v>
       </c>
       <c r="D17" t="n">
-        <v>0.100523141253148</v>
+        <v>0.108567315464557</v>
       </c>
       <c r="E17" t="n">
-        <v>1.2493706145333</v>
+        <v>0.302016972119236</v>
       </c>
       <c r="F17" t="n">
-        <v>0.98423255202759</v>
+        <v>0.268942034375936</v>
       </c>
       <c r="G17" t="n">
-        <v>0.478745908392527</v>
+        <v>0.0579194505926401</v>
       </c>
     </row>
     <row r="18">
@@ -958,22 +922,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>0.405518674764158</v>
+        <v>3.6754884764588</v>
       </c>
       <c r="C18" t="n">
-        <v>0.328764175247605</v>
+        <v>0.849081646660459</v>
       </c>
       <c r="D18" t="n">
-        <v>1.01767287557923</v>
+        <v>0.0372227680258674</v>
       </c>
       <c r="E18" t="n">
-        <v>0.412199423008007</v>
+        <v>0.145837459578544</v>
       </c>
       <c r="F18" t="n">
-        <v>0.371309888522239</v>
+        <v>0.139647703717015</v>
       </c>
       <c r="G18" t="n">
-        <v>0.236032866463292</v>
+        <v>0.0620565542064001</v>
       </c>
     </row>
     <row r="19">
@@ -981,22 +945,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>0.123771340504966</v>
+        <v>0.310314137532402</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0968887310911481</v>
+        <v>0.302009022107109</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0143704862062098</v>
+        <v>5.03955283928082</v>
       </c>
       <c r="E19" t="n">
-        <v>0.410054112404886</v>
+        <v>0.231684520472518</v>
       </c>
       <c r="F19" t="n">
-        <v>1.07313966772049</v>
+        <v>0.268946378454534</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0155870760871986</v>
+        <v>3.10696481393376</v>
       </c>
     </row>
     <row r="20">
@@ -1004,22 +968,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>0.163547756557875</v>
+        <v>1.44310820523797</v>
       </c>
       <c r="C20" t="n">
-        <v>0.423688136441397</v>
+        <v>1.37555522386388</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0762424625032548</v>
+        <v>5.62269125699535</v>
       </c>
       <c r="E20" t="n">
-        <v>3.80683112818364</v>
+        <v>3.05017048345841</v>
       </c>
       <c r="F20" t="n">
-        <v>4.56529144833926</v>
+        <v>1.57020962272951</v>
       </c>
       <c r="G20" t="n">
-        <v>0.153644035716671</v>
+        <v>4.81145150280289</v>
       </c>
     </row>
     <row r="21">
@@ -1027,22 +991,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>4.68403542260676</v>
+        <v>1.25061704022951</v>
       </c>
       <c r="C21" t="n">
-        <v>6.26778039490037</v>
+        <v>1.47688566272041</v>
       </c>
       <c r="D21" t="n">
-        <v>1.0883717562809</v>
+        <v>0.454943980361674</v>
       </c>
       <c r="E21" t="n">
-        <v>4.20746391344146</v>
+        <v>0.848132278857342</v>
       </c>
       <c r="F21" t="n">
-        <v>4.70677499231295</v>
+        <v>1.10680099383993</v>
       </c>
       <c r="G21" t="n">
-        <v>2.09312164599524</v>
+        <v>1.08392114680512</v>
       </c>
     </row>
     <row r="22">
@@ -1050,22 +1014,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>0.62203235747903</v>
+        <v>2.5768893369916</v>
       </c>
       <c r="C22" t="n">
-        <v>0.530378953047369</v>
+        <v>2.89477196547078</v>
       </c>
       <c r="D22" t="n">
-        <v>1.0089229250021</v>
+        <v>1.3214054852967</v>
       </c>
       <c r="E22" t="n">
-        <v>0.572820714663906</v>
+        <v>2.64473306730114</v>
       </c>
       <c r="F22" t="n">
-        <v>0.555796676841172</v>
+        <v>2.17118728162804</v>
       </c>
       <c r="G22" t="n">
-        <v>0.331782048141798</v>
+        <v>1.24733673954864</v>
       </c>
     </row>
     <row r="23">
@@ -1073,22 +1037,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>0.489431539055436</v>
+        <v>0.597929761258555</v>
       </c>
       <c r="C23" t="n">
-        <v>1.03557858060559</v>
+        <v>0.689822641970843</v>
       </c>
       <c r="D23" t="n">
-        <v>0.116057215244497</v>
+        <v>1.1797556481697</v>
       </c>
       <c r="E23" t="n">
-        <v>0.324532648064848</v>
+        <v>0.5078458359878</v>
       </c>
       <c r="F23" t="n">
-        <v>0.285592193269387</v>
+        <v>0.607182372697673</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0623483043487942</v>
+        <v>0.872928862503361</v>
       </c>
     </row>
     <row r="24">
@@ -1096,22 +1060,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>0.423254220084809</v>
+        <v>0.479989679078026</v>
       </c>
       <c r="C24" t="n">
-        <v>0.368963821508924</v>
+        <v>0.778767248922643</v>
       </c>
       <c r="D24" t="n">
-        <v>0.272935517541799</v>
+        <v>0.370161031603955</v>
       </c>
       <c r="E24" t="n">
-        <v>0.813106647452669</v>
+        <v>1.00121302890389</v>
       </c>
       <c r="F24" t="n">
-        <v>0.603027868696072</v>
+        <v>0.819235231134474</v>
       </c>
       <c r="G24" t="n">
-        <v>0.612349417711372</v>
+        <v>1.21837701425232</v>
       </c>
     </row>
     <row r="25">
@@ -1119,22 +1083,22 @@
         <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>0.00992085363433938</v>
+        <v>7.86277831879809</v>
       </c>
       <c r="C25" t="n">
-        <v>0.012243625528391</v>
+        <v>7.84790848346589</v>
       </c>
       <c r="D25" t="n">
-        <v>1.17798840813456</v>
+        <v>0.432196947051801</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00553464688952845</v>
+        <v>1.98483061553141</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0109759845458138</v>
+        <v>1.75330185731821</v>
       </c>
       <c r="G25" t="n">
-        <v>0.621256318332628</v>
+        <v>0.324762633680161</v>
       </c>
     </row>
     <row r="26">
@@ -1142,22 +1106,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>3.92694325048742</v>
+        <v>0.317577226213448</v>
       </c>
       <c r="C26" t="n">
-        <v>0.91547529392264</v>
+        <v>0.274071527502904</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0397812945553747</v>
+        <v>0.331901999266351</v>
       </c>
       <c r="E26" t="n">
-        <v>0.156550024538266</v>
+        <v>0.755047426231547</v>
       </c>
       <c r="F26" t="n">
-        <v>0.148236503625262</v>
+        <v>0.495472208820514</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0668017546594224</v>
+        <v>0.552303332436961</v>
       </c>
     </row>
     <row r="27">
@@ -1165,22 +1129,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>0.33137348514043</v>
+        <v>0.395164235637485</v>
       </c>
       <c r="C27" t="n">
-        <v>0.325323728548659</v>
+        <v>0.402321764763826</v>
       </c>
       <c r="D27" t="n">
-        <v>5.38605902624574</v>
+        <v>1.30796227309414</v>
       </c>
       <c r="E27" t="n">
-        <v>0.248870725896926</v>
+        <v>1.07775226994655</v>
       </c>
       <c r="F27" t="n">
-        <v>0.285544607987049</v>
+        <v>0.630977245111131</v>
       </c>
       <c r="G27" t="n">
-        <v>3.34454118328175</v>
+        <v>1.57830502864944</v>
       </c>
     </row>
     <row r="28">
@@ -1188,22 +1152,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>1.54193379355456</v>
+        <v>1.36337371460772</v>
       </c>
       <c r="C28" t="n">
-        <v>1.48222164534777</v>
+        <v>1.93273425562217</v>
       </c>
       <c r="D28" t="n">
-        <v>6.00872717263494</v>
+        <v>0.0961579086777135</v>
       </c>
       <c r="E28" t="n">
-        <v>3.27565889026833</v>
+        <v>2.40478240584764</v>
       </c>
       <c r="F28" t="n">
-        <v>1.66739823488254</v>
+        <v>3.77758412764654</v>
       </c>
       <c r="G28" t="n">
-        <v>5.17936271126055</v>
+        <v>0.24202056140496</v>
       </c>
     </row>
     <row r="29">
@@ -1211,22 +1175,22 @@
         <v>34</v>
       </c>
       <c r="B29" t="n">
-        <v>0.235335133073849</v>
+        <v>0.183099856577867</v>
       </c>
       <c r="C29" t="n">
-        <v>0.21620553341772</v>
+        <v>0.19339796183196</v>
       </c>
       <c r="D29" t="n">
-        <v>0.842107663612419</v>
+        <v>0.375327385969445</v>
       </c>
       <c r="E29" t="n">
-        <v>0.104291280057551</v>
+        <v>0.230650886445782</v>
       </c>
       <c r="F29" t="n">
-        <v>0.126309147610706</v>
+        <v>0.228600609382895</v>
       </c>
       <c r="G29" t="n">
-        <v>1.01315994566791</v>
+        <v>1.27836501665184</v>
       </c>
     </row>
     <row r="30">
@@ -1234,22 +1198,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="n">
-        <v>1.47172192328023</v>
+        <v>1.02201306234004</v>
       </c>
       <c r="C30" t="n">
-        <v>1.76004654858446</v>
+        <v>1.25558730210335</v>
       </c>
       <c r="D30" t="n">
-        <v>0.52596031289439</v>
+        <v>1.06187916617168</v>
       </c>
       <c r="E30" t="n">
-        <v>0.99500992133414</v>
+        <v>1.63007017249191</v>
       </c>
       <c r="F30" t="n">
-        <v>1.30053452981999</v>
+        <v>1.24230573053892</v>
       </c>
       <c r="G30" t="n">
-        <v>1.27814023915028</v>
+        <v>0.415778913182881</v>
       </c>
     </row>
     <row r="31">
@@ -1257,22 +1221,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0917056732680476</v>
+        <v>0.0279289195628604</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0924777006840251</v>
+        <v>0.138609041509549</v>
       </c>
       <c r="D31" t="n">
-        <v>0.127060733382998</v>
+        <v>0.0682419551978026</v>
       </c>
       <c r="E31" t="n">
-        <v>0.089860069253163</v>
+        <v>0.225478308764813</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0746760758348479</v>
+        <v>0.0951640606850164</v>
       </c>
       <c r="G31" t="n">
-        <v>1.43401100002227</v>
+        <v>2.14715677554144</v>
       </c>
     </row>
     <row r="32">
@@ -1280,22 +1244,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>2.75326270771866</v>
+        <v>0.630995090669457</v>
       </c>
       <c r="C32" t="n">
-        <v>3.12064386399474</v>
+        <v>0.627753827598814</v>
       </c>
       <c r="D32" t="n">
-        <v>1.41214896543255</v>
+        <v>0.90161858648288</v>
       </c>
       <c r="E32" t="n">
-        <v>2.83677283305925</v>
+        <v>0.220307143210645</v>
       </c>
       <c r="F32" t="n">
-        <v>2.30563457945906</v>
+        <v>0.422030937856687</v>
       </c>
       <c r="G32" t="n">
-        <v>1.34271526865439</v>
+        <v>2.24851581407856</v>
       </c>
     </row>
     <row r="33">
@@ -1303,22 +1267,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="n">
-        <v>0.648799795781567</v>
+        <v>0.251366439731879</v>
       </c>
       <c r="C33" t="n">
-        <v>0.743644412363356</v>
+        <v>0.21305750514979</v>
       </c>
       <c r="D33" t="n">
-        <v>1.2697047198946</v>
+        <v>1.11978296030384</v>
       </c>
       <c r="E33" t="n">
-        <v>0.559421030269464</v>
+        <v>0.299948698460315</v>
       </c>
       <c r="F33" t="n">
-        <v>0.674504678860047</v>
+        <v>0.317555911781794</v>
       </c>
       <c r="G33" t="n">
-        <v>0.970852167716939</v>
+        <v>0.299940011997601</v>
       </c>
     </row>
     <row r="34">
@@ -1326,22 +1290,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>0.512788083276204</v>
+        <v>8.92097430572145</v>
       </c>
       <c r="C34" t="n">
-        <v>0.839501193295725</v>
+        <v>4.24562353452689</v>
       </c>
       <c r="D34" t="n">
-        <v>0.395643023457045</v>
+        <v>10.4978821849263</v>
       </c>
       <c r="E34" t="n">
-        <v>1.0738999683416</v>
+        <v>2.2537537969811</v>
       </c>
       <c r="F34" t="n">
-        <v>0.869996987417279</v>
+        <v>2.85181901426348</v>
       </c>
       <c r="G34" t="n">
-        <v>1.31154111647999</v>
+        <v>4.89419357507809</v>
       </c>
     </row>
     <row r="35">
@@ -1349,22 +1313,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="n">
-        <v>1.09173160281349</v>
+        <v>0.63202530038048</v>
       </c>
       <c r="C35" t="n">
-        <v>1.2389645879585</v>
+        <v>0.568836660325994</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0331544246147323</v>
+        <v>0.506641200201262</v>
       </c>
       <c r="E35" t="n">
-        <v>0.263281372255507</v>
+        <v>0.891575653831975</v>
       </c>
       <c r="F35" t="n">
-        <v>0.263627097203321</v>
+        <v>0.674425221286529</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0578948540381661</v>
+        <v>0.616428438450241</v>
       </c>
     </row>
     <row r="36">
@@ -1372,22 +1336,22 @@
         <v>41</v>
       </c>
       <c r="B36" t="n">
-        <v>8.39911220870484</v>
+        <v>2.4154662595499</v>
       </c>
       <c r="C36" t="n">
-        <v>8.45641336492007</v>
+        <v>2.27640252437639</v>
       </c>
       <c r="D36" t="n">
-        <v>0.461881610496188</v>
+        <v>3.61888396653541</v>
       </c>
       <c r="E36" t="n">
-        <v>2.13283454344001</v>
+        <v>2.2423800784114</v>
       </c>
       <c r="F36" t="n">
-        <v>1.86176833190812</v>
+        <v>3.29658459116357</v>
       </c>
       <c r="G36" t="n">
-        <v>0.34959584938431</v>
+        <v>5.19206503526881</v>
       </c>
     </row>
     <row r="37">
@@ -1395,22 +1359,22 @@
         <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>0.624384699909399</v>
+        <v>0.154119924930775</v>
       </c>
       <c r="C37" t="n">
-        <v>0.75559536712734</v>
+        <v>0.145835110253019</v>
       </c>
       <c r="D37" t="n">
-        <v>0.354684757842184</v>
+        <v>2.17753994765246</v>
       </c>
       <c r="E37" t="n">
-        <v>0.840725043378159</v>
+        <v>0.0537839088306768</v>
       </c>
       <c r="F37" t="n">
-        <v>0.588773856632756</v>
+        <v>0.0879245788041524</v>
       </c>
       <c r="G37" t="n">
-        <v>0.632389944109199</v>
+        <v>1.25767949858304</v>
       </c>
     </row>
     <row r="38">
@@ -1418,22 +1382,22 @@
         <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>0.422168315046483</v>
+        <v>10.1323917562282</v>
       </c>
       <c r="C38" t="n">
-        <v>0.433551588406822</v>
+        <v>9.44676400137237</v>
       </c>
       <c r="D38" t="n">
-        <v>1.39773163776612</v>
+        <v>2.37087481704744</v>
       </c>
       <c r="E38" t="n">
-        <v>1.15592241935093</v>
+        <v>9.83624880476411</v>
       </c>
       <c r="F38" t="n">
-        <v>0.670066699759383</v>
+        <v>13.1171043231126</v>
       </c>
       <c r="G38" t="n">
-        <v>1.69899129350464</v>
+        <v>3.94265974391329</v>
       </c>
     </row>
     <row r="39">
@@ -1441,22 +1405,22 @@
         <v>44</v>
       </c>
       <c r="B39" t="n">
-        <v>0.99006678116941</v>
+        <v>0.280330191755365</v>
       </c>
       <c r="C39" t="n">
-        <v>2.1064472429772</v>
+        <v>0.294767678614598</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0817559319375589</v>
+        <v>1.56645671115686</v>
       </c>
       <c r="E39" t="n">
-        <v>1.8522226200974</v>
+        <v>0.0589555664896391</v>
       </c>
       <c r="F39" t="n">
-        <v>4.2796401836849</v>
+        <v>0.0672370065521211</v>
       </c>
       <c r="G39" t="n">
-        <v>0.182591462735755</v>
+        <v>0.13031876383344</v>
       </c>
     </row>
     <row r="40">
@@ -1464,22 +1428,22 @@
         <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>0.879534186865</v>
+        <v>1.52382744854149</v>
       </c>
       <c r="C40" t="n">
-        <v>0.918599467376178</v>
+        <v>1.56686869588858</v>
       </c>
       <c r="D40" t="n">
-        <v>0.405536486907794</v>
+        <v>1.01018654339857</v>
       </c>
       <c r="E40" t="n">
-        <v>0.503406340173492</v>
+        <v>2.22790537217804</v>
       </c>
       <c r="F40" t="n">
-        <v>0.666716473882472</v>
+        <v>1.77811442109062</v>
       </c>
       <c r="G40" t="n">
-        <v>0.489879534169098</v>
+        <v>2.27333843576112</v>
       </c>
     </row>
     <row r="41">
@@ -1487,22 +1451,22 @@
         <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>1.45626213090655</v>
+        <v>0.0868989606531248</v>
       </c>
       <c r="C41" t="n">
-        <v>2.08658240117844</v>
+        <v>0.1778888502191</v>
       </c>
       <c r="D41" t="n">
-        <v>0.102739904810064</v>
+        <v>0.309155179773523</v>
       </c>
       <c r="E41" t="n">
-        <v>2.57635272973834</v>
+        <v>1.0146543792567</v>
       </c>
       <c r="F41" t="n">
-        <v>4.01165879184296</v>
+        <v>0.356866762975902</v>
       </c>
       <c r="G41" t="n">
-        <v>0.260526843171747</v>
+        <v>0.0496452433651201</v>
       </c>
     </row>
     <row r="42">
@@ -1510,22 +1474,22 @@
         <v>47</v>
       </c>
       <c r="B42" t="n">
-        <v>0.195613423794794</v>
+        <v>0.10551284715383</v>
       </c>
       <c r="C42" t="n">
-        <v>0.208495671197655</v>
+        <v>0.145834019199516</v>
       </c>
       <c r="D42" t="n">
-        <v>0.401059464152334</v>
+        <v>0.883007095561423</v>
       </c>
       <c r="E42" t="n">
-        <v>0.247544442430411</v>
+        <v>1.51525735269371</v>
       </c>
       <c r="F42" t="n">
-        <v>0.242754676976423</v>
+        <v>1.2060973860402</v>
       </c>
       <c r="G42" t="n">
-        <v>1.3761161459841</v>
+        <v>1.085989698612</v>
       </c>
     </row>
     <row r="43">
@@ -1533,22 +1497,22 @@
         <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>1.09164407197533</v>
+        <v>1.61071947507021</v>
       </c>
       <c r="C43" t="n">
-        <v>1.35287617368877</v>
+        <v>1.76956994258125</v>
       </c>
       <c r="D43" t="n">
-        <v>1.13475650004681</v>
+        <v>0.370160390152818</v>
       </c>
       <c r="E43" t="n">
-        <v>1.74967552066169</v>
+        <v>1.34667326901845</v>
       </c>
       <c r="F43" t="n">
-        <v>1.31921175313772</v>
+        <v>1.22471632090368</v>
       </c>
       <c r="G43" t="n">
-        <v>0.44757175621813</v>
+        <v>0.378544980659041</v>
       </c>
     </row>
     <row r="44">
@@ -1556,22 +1520,22 @@
         <v>49</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0298282090316424</v>
+        <v>0.906179627077576</v>
       </c>
       <c r="C44" t="n">
-        <v>0.149086537078452</v>
+        <v>1.10872067563948</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0729390649886937</v>
+        <v>1.74947159393509</v>
       </c>
       <c r="E44" t="n">
-        <v>0.242325117043258</v>
+        <v>2.05310159740289</v>
       </c>
       <c r="F44" t="n">
-        <v>0.101056178796311</v>
+        <v>2.34081704544745</v>
       </c>
       <c r="G44" t="n">
-        <v>2.31134071121601</v>
+        <v>2.04579773700432</v>
       </c>
     </row>
     <row r="45">
@@ -1579,22 +1543,22 @@
         <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>0.673956144016784</v>
+        <v>0.996173069155104</v>
       </c>
       <c r="C45" t="n">
-        <v>0.683628172743384</v>
+        <v>1.11697062321928</v>
       </c>
       <c r="D45" t="n">
-        <v>1.01112630528467</v>
+        <v>0.358786606226575</v>
       </c>
       <c r="E45" t="n">
-        <v>0.236653373848349</v>
+        <v>0.407516708684414</v>
       </c>
       <c r="F45" t="n">
-        <v>0.448172956907226</v>
+        <v>0.542019995366653</v>
       </c>
       <c r="G45" t="n">
-        <v>2.53623995190274</v>
+        <v>0.471629811968641</v>
       </c>
     </row>
     <row r="46">
@@ -1602,22 +1566,22 @@
         <v>51</v>
       </c>
       <c r="B46" t="n">
-        <v>0.279542700118227</v>
+        <v>0.945483999124638</v>
       </c>
       <c r="C46" t="n">
-        <v>0.252960012483894</v>
+        <v>0.662930847273026</v>
       </c>
       <c r="D46" t="n">
-        <v>1.22874310846116</v>
+        <v>0.0744448946005979</v>
       </c>
       <c r="E46" t="n">
-        <v>0.394433714439364</v>
+        <v>1.36114859573177</v>
       </c>
       <c r="F46" t="n">
-        <v>0.409747165766049</v>
+        <v>1.17920480039739</v>
       </c>
       <c r="G46" t="n">
-        <v>0.509920060566924</v>
+        <v>0.335105392714561</v>
       </c>
     </row>
     <row r="47">
@@ -1625,22 +1589,22 @@
         <v>52</v>
       </c>
       <c r="B47" t="n">
-        <v>1.69753556216887</v>
+        <v>1.00134723145823</v>
       </c>
       <c r="C47" t="n">
-        <v>1.45646641932221</v>
+        <v>0.981492498792379</v>
       </c>
       <c r="D47" t="n">
-        <v>3.15721320554993</v>
+        <v>0.375329203414333</v>
       </c>
       <c r="E47" t="n">
-        <v>1.54784421385832</v>
+        <v>0.879160919663618</v>
       </c>
       <c r="F47" t="n">
-        <v>2.0344375132282</v>
+        <v>1.03542551414419</v>
       </c>
       <c r="G47" t="n">
-        <v>3.48705159322185</v>
+        <v>0.852243344434561</v>
       </c>
     </row>
     <row r="48">
@@ -1648,22 +1612,22 @@
         <v>53</v>
       </c>
       <c r="B48" t="n">
-        <v>9.52927173001842</v>
+        <v>1.17718168798025</v>
       </c>
       <c r="C48" t="n">
-        <v>4.57458193586273</v>
+        <v>1.20902068933866</v>
       </c>
       <c r="D48" t="n">
-        <v>11.2202949946802</v>
+        <v>0.514914209331506</v>
       </c>
       <c r="E48" t="n">
-        <v>2.42053335946645</v>
+        <v>0.563696285412688</v>
       </c>
       <c r="F48" t="n">
-        <v>3.02838600503835</v>
+        <v>0.762349500499054</v>
       </c>
       <c r="G48" t="n">
-        <v>5.26843171747311</v>
+        <v>0.897751484185922</v>
       </c>
     </row>
     <row r="49">
@@ -1671,22 +1635,22 @@
         <v>54</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0861612638513247</v>
+        <v>0.138612076728478</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0902344215108627</v>
+        <v>0.198572636057761</v>
       </c>
       <c r="D49" t="n">
-        <v>0.994498905698501</v>
+        <v>1.1601106725581</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0311516833325472</v>
+        <v>0.178934716377511</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0417349952229685</v>
+        <v>0.173778572874174</v>
       </c>
       <c r="G49" t="n">
-        <v>0.0133603509318845</v>
+        <v>0.515069399913121</v>
       </c>
     </row>
     <row r="50">
@@ -1694,22 +1658,22 @@
         <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>0.681645010123232</v>
+        <v>0.160331231069324</v>
       </c>
       <c r="C50" t="n">
-        <v>0.612974319781168</v>
+        <v>0.233740927303949</v>
       </c>
       <c r="D50" t="n">
-        <v>0.541404049783897</v>
+        <v>2.49289550102423</v>
       </c>
       <c r="E50" t="n">
-        <v>0.956435212793488</v>
+        <v>0.334081643288638</v>
       </c>
       <c r="F50" t="n">
-        <v>0.716162553108191</v>
+        <v>0.293773622216689</v>
       </c>
       <c r="G50" t="n">
-        <v>0.663564096283596</v>
+        <v>7.73845230953809</v>
       </c>
     </row>
     <row r="51">
@@ -1717,22 +1681,22 @@
         <v>56</v>
       </c>
       <c r="B51" t="n">
-        <v>0.20892328880136</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0.292900031454207</v>
+        <v>0.0113768641329402</v>
       </c>
       <c r="D51" t="n">
-        <v>1.05311098012261</v>
+        <v>0.0516982889248159</v>
       </c>
       <c r="E51" t="n">
-        <v>0.241197623219546</v>
+        <v>0.012411824331313</v>
       </c>
       <c r="F51" t="n">
-        <v>0.426201297353941</v>
+        <v>0.0124136218810775</v>
       </c>
       <c r="G51" t="n">
-        <v>0.249393217395177</v>
+        <v>1.22251411786608</v>
       </c>
     </row>
     <row r="52">
@@ -1740,22 +1704,22 @@
         <v>57</v>
       </c>
       <c r="B52" t="n">
-        <v>0.882988846365851</v>
+        <v>0.256529815619265</v>
       </c>
       <c r="C52" t="n">
-        <v>0.996264549120842</v>
+        <v>0.385781500624617</v>
       </c>
       <c r="D52" t="n">
-        <v>0.71052975765092</v>
+        <v>1.32968009805479</v>
       </c>
       <c r="E52" t="n">
-        <v>0.845975338722066</v>
+        <v>1.13567152792687</v>
       </c>
       <c r="F52" t="n">
-        <v>1.41599896262926</v>
+        <v>0.921640271658491</v>
       </c>
       <c r="G52" t="n">
-        <v>2.10202854661649</v>
+        <v>1.49763150818112</v>
       </c>
     </row>
     <row r="53">
@@ -1763,22 +1727,22 @@
         <v>58</v>
       </c>
       <c r="B53" t="n">
-        <v>0.163460225719709</v>
+        <v>1.71200207830604</v>
       </c>
       <c r="C53" t="n">
-        <v>0.154841070393562</v>
+        <v>1.49656193552529</v>
       </c>
       <c r="D53" t="n">
-        <v>2.18266517186368</v>
+        <v>1.57369292143276</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0522039059585625</v>
+        <v>2.05724464906236</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0911564613716162</v>
+        <v>1.84535382437576</v>
       </c>
       <c r="G53" t="n">
-        <v>1.29372731523748</v>
+        <v>2.09337442856256</v>
       </c>
     </row>
     <row r="54">
@@ -1786,22 +1750,22 @@
         <v>59</v>
       </c>
       <c r="B54" t="n">
-        <v>9.16298516332999</v>
+        <v>2.08856013202549</v>
       </c>
       <c r="C54" t="n">
-        <v>7.29183862937429</v>
+        <v>2.22157796297289</v>
       </c>
       <c r="D54" t="n">
-        <v>1.63747927250732</v>
+        <v>0.247116484704084</v>
       </c>
       <c r="E54" t="n">
-        <v>7.59853185440546</v>
+        <v>0.590590882216813</v>
       </c>
       <c r="F54" t="n">
-        <v>8.84251491742136</v>
+        <v>0.642364337680245</v>
       </c>
       <c r="G54" t="n">
-        <v>2.18441737736311</v>
+        <v>0.26270607947376</v>
       </c>
     </row>
     <row r="55">
@@ -1809,298 +1773,22 @@
         <v>60</v>
       </c>
       <c r="B55" t="n">
-        <v>1.63386923527279</v>
+        <v>25.9792225699503</v>
       </c>
       <c r="C55" t="n">
-        <v>1.67757391475186</v>
+        <v>29.2051758920982</v>
       </c>
       <c r="D55" t="n">
-        <v>1.04982431170098</v>
+        <v>31.1327052072747</v>
       </c>
       <c r="E55" t="n">
-        <v>2.35091639806147</v>
+        <v>31.2857438231278</v>
       </c>
       <c r="F55" t="n">
-        <v>1.87728074786288</v>
+        <v>29.1772120315926</v>
       </c>
       <c r="G55" t="n">
-        <v>2.40931661804983</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" t="n">
-        <v>0.216666861681662</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.332129094007348</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1.13601711657096</v>
-      </c>
-      <c r="E56" t="n">
-        <v>1.83227047203402</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.610712698749946</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0.104656082299762</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" t="n">
-        <v>0.112709875058447</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0.157079629070524</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.898399254103426</v>
-      </c>
-      <c r="E57" t="n">
-        <v>1.62790998497247</v>
-      </c>
-      <c r="F57" t="n">
-        <v>1.28081713856084</v>
-      </c>
-      <c r="G57" t="n">
-        <v>1.16903070653989</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" t="n">
-        <v>1.71122837459241</v>
-      </c>
-      <c r="C58" t="n">
-        <v>1.90728632817056</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.377949064824754</v>
-      </c>
-      <c r="E58" t="n">
-        <v>1.42988921573043</v>
-      </c>
-      <c r="F58" t="n">
-        <v>1.27093054811058</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.376316551248079</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" t="n">
-        <v>0.968053263824079</v>
-      </c>
-      <c r="C59" t="n">
-        <v>1.19466074354307</v>
-      </c>
-      <c r="D59" t="n">
-        <v>1.86976768556283</v>
-      </c>
-      <c r="E59" t="n">
-        <v>2.20398624373699</v>
-      </c>
-      <c r="F59" t="n">
-        <v>2.48589342026834</v>
-      </c>
-      <c r="G59" t="n">
-        <v>2.20223117860562</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" t="n">
-        <v>1.06970714411339</v>
-      </c>
-      <c r="C60" t="n">
-        <v>1.0577800680234</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0.401116343068308</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.944084315135209</v>
-      </c>
-      <c r="F60" t="n">
-        <v>1.09954438375902</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0.917410763989401</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" t="n">
-        <v>0.148049669442501</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0.214023620695159</v>
-      </c>
-      <c r="D61" t="n">
-        <v>1.23988380516171</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.192273376503086</v>
-      </c>
-      <c r="F61" t="n">
-        <v>0.184529450985857</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0.554454563673206</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" t="n">
-        <v>0.171225681309553</v>
-      </c>
-      <c r="C62" t="n">
-        <v>0.251866695874513</v>
-      </c>
-      <c r="D62" t="n">
-        <v>2.66436716744724</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.35859383061497</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.311886970897002</v>
-      </c>
-      <c r="G62" t="n">
-        <v>8.33017880602997</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" t="n">
-        <v>0</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0.0122577870169913</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0.055251797993576</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.0132831525348683</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.0131711814549765</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1.31599456679062</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" t="n">
-        <v>0.240797482329791</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0.365495051832777</v>
-      </c>
-      <c r="D64" t="n">
-        <v>1.15031399476827</v>
-      </c>
-      <c r="E64" t="n">
-        <v>1.08548337326584</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0.839224849765687</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1.12449620343361</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" t="n">
-        <v>1.8288042950718</v>
-      </c>
-      <c r="C65" t="n">
-        <v>1.61262266964655</v>
-      </c>
-      <c r="D65" t="n">
-        <v>1.68177104800403</v>
-      </c>
-      <c r="E65" t="n">
-        <v>2.20656316112597</v>
-      </c>
-      <c r="F65" t="n">
-        <v>1.95962688590536</v>
-      </c>
-      <c r="G65" t="n">
-        <v>2.25344585717785</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" t="n">
-        <v>1.62996050954895</v>
-      </c>
-      <c r="C66" t="n">
-        <v>1.52362790012728</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0.259641627837473</v>
-      </c>
-      <c r="E66" t="n">
-        <v>1.13681341356564</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.959926221461738</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0.331782048141798</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>72</v>
-      </c>
-      <c r="B67" t="n">
-        <v>19.2749641900815</v>
-      </c>
-      <c r="C67" t="n">
-        <v>22.2655926009364</v>
-      </c>
-      <c r="D67" t="n">
-        <v>20.601882245977</v>
-      </c>
-      <c r="E67" t="n">
-        <v>22.7419234939098</v>
-      </c>
-      <c r="F67" t="n">
-        <v>22.3080097993096</v>
-      </c>
-      <c r="G67" t="n">
-        <v>20.1674497316796</v>
+        <v>29.0383302649815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>